<commit_message>
added decision table (control-break) against review comments #70
</commit_message>
<xml_diff>
--- a/migration/TERASOLUNA3.3.1移行ガイド_図.xlsx
+++ b/migration/TERASOLUNA3.3.1移行ガイド_図.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="1260" windowWidth="17235" windowHeight="8955"/>
+    <workbookView xWindow="-75" yWindow="1260" windowWidth="17235" windowHeight="8955" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="batch " sheetId="13" r:id="rId1"/>
+    <sheet name="コントロールブレイク" sheetId="14" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'batch '!$A$1:$C$1</definedName>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="69">
   <si>
     <t>種別</t>
     <rPh sb="0" eb="2">
@@ -265,12 +266,61 @@
     <t>3.3.1のライブラリ</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>拡張入力チェックエラーハンドラの実装</t>
+  </si>
+  <si>
+    <t>例外をスローする（拡張入力チェックエラーハンドラを実装しない場合を含む）</t>
+  </si>
+  <si>
+    <t>○</t>
+  </si>
+  <si>
+    <t>当該データの取得をスキップする</t>
+  </si>
+  <si>
+    <t>入力データの取得を終了する</t>
+  </si>
+  <si>
+    <t>拡張例外ハンドラの実装</t>
+  </si>
+  <si>
+    <t>発生した例外をそのままスローする（拡張例外ハンドラを実装しない場合を含む）</t>
+  </si>
+  <si>
+    <t>例外発生データの種類</t>
+  </si>
+  <si>
+    <t>入力チェックエラーが発生</t>
+  </si>
+  <si>
+    <t>データの入力時に例外が発生</t>
+  </si>
+  <si>
+    <t>例外発生データ検出時の振舞い</t>
+  </si>
+  <si>
+    <t>パターン1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>パターン2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>パターン3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>パターン4</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,8 +375,36 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="ＭＳ Ｐ明朝"/>
+      <family val="1"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐ明朝"/>
+      <family val="1"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="ＭＳ 明朝"/>
+      <family val="1"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="ＭＳ Ｐ明朝"/>
+      <family val="1"/>
+      <charset val="128"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -339,8 +417,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000099"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -363,13 +447,89 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalDown="1">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="thin">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
+    <border diagonalDown="1">
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="thin">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -399,6 +559,54 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -706,8 +914,8 @@
   </sheetPr>
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -998,4 +1206,560 @@
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:T13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X6" sqref="X6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="16.625" customWidth="1"/>
+    <col min="2" max="2" width="15.625" customWidth="1"/>
+    <col min="3" max="3" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" s="10"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="16">
+        <v>1</v>
+      </c>
+      <c r="D1" s="17"/>
+      <c r="E1" s="16">
+        <v>2</v>
+      </c>
+      <c r="F1" s="17"/>
+      <c r="G1" s="16">
+        <v>3</v>
+      </c>
+      <c r="H1" s="17"/>
+      <c r="I1" s="16">
+        <v>4</v>
+      </c>
+      <c r="J1" s="17"/>
+      <c r="K1" s="16">
+        <v>5</v>
+      </c>
+      <c r="L1" s="17"/>
+      <c r="M1" s="16">
+        <v>6</v>
+      </c>
+      <c r="N1" s="17"/>
+      <c r="O1" s="16">
+        <v>7</v>
+      </c>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="16">
+        <v>8</v>
+      </c>
+      <c r="R1" s="17"/>
+      <c r="S1" s="16">
+        <v>9</v>
+      </c>
+      <c r="T1" s="17"/>
+    </row>
+    <row r="2" spans="1:20" ht="48">
+      <c r="A2" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="19"/>
+      <c r="E2" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="19"/>
+      <c r="G2" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="19"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="19"/>
+    </row>
+    <row r="3" spans="1:20" ht="24">
+      <c r="A3" s="25"/>
+      <c r="B3" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="J3" s="21"/>
+      <c r="K3" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="L3" s="21"/>
+      <c r="M3" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="N3" s="21"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="21"/>
+    </row>
+    <row r="4" spans="1:20" ht="24">
+      <c r="A4" s="25"/>
+      <c r="B4" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="R4" s="21"/>
+      <c r="S4" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="T4" s="21"/>
+    </row>
+    <row r="5" spans="1:20" ht="48">
+      <c r="A5" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="J5" s="19"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="18"/>
+      <c r="T5" s="19"/>
+    </row>
+    <row r="6" spans="1:20" ht="24">
+      <c r="A6" s="25"/>
+      <c r="B6" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="21"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="L6" s="19"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="R6" s="19"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="21"/>
+    </row>
+    <row r="7" spans="1:20" ht="24">
+      <c r="A7" s="25"/>
+      <c r="B7" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="21"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="N7" s="19"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="T7" s="19"/>
+    </row>
+    <row r="8" spans="1:20" ht="24">
+      <c r="A8" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="T8" s="12"/>
+    </row>
+    <row r="9" spans="1:20" ht="24">
+      <c r="A9" s="24"/>
+      <c r="B9" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="23"/>
+      <c r="B11" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="23"/>
+      <c r="B12" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="J12" s="13"/>
+      <c r="K12" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="N12" s="13"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="S12" s="12"/>
+      <c r="T12" s="13"/>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="23"/>
+      <c r="B13" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="I13" s="13"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="O13" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="T13" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="68">
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+  </mergeCells>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="94" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
modified decision table layout and removed AL-042 note #70
</commit_message>
<xml_diff>
--- a/migration/TERASOLUNA3.3.1移行ガイド_図.xlsx
+++ b/migration/TERASOLUNA3.3.1移行ガイド_図.xlsx
@@ -288,18 +288,12 @@
     <t>発生した例外をそのままスローする（拡張例外ハンドラを実装しない場合を含む）</t>
   </si>
   <si>
-    <t>例外発生データの種類</t>
-  </si>
-  <si>
     <t>入力チェックエラーが発生</t>
   </si>
   <si>
     <t>データの入力時に例外が発生</t>
   </si>
   <si>
-    <t>例外発生データ検出時の振舞い</t>
-  </si>
-  <si>
     <t>パターン1</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -313,6 +307,23 @@
   </si>
   <si>
     <t>パターン4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>異常データの種類</t>
+    <rPh sb="0" eb="2">
+      <t>イジョウ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>シュルイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>異常データ検出時の振る舞い</t>
+    <rPh sb="0" eb="2">
+      <t>イジョウ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -424,7 +435,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -449,45 +460,158 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000099"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000099"/>
+      </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000099"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000099"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalDown="1">
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000099"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal style="thin">
+        <color theme="0"/>
+      </diagonal>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000099"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000099"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000099"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000099"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000099"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000099"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000099"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000099"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000099"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000099"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000099"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000099"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000099"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000099"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000099"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000099"/>
       </right>
       <top/>
       <bottom/>
@@ -495,33 +619,40 @@
     </border>
     <border diagonalDown="1">
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000099"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000099"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal style="thin">
-        <color indexed="64"/>
+        <color theme="0"/>
       </diagonal>
     </border>
     <border diagonalDown="1">
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color theme="0"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000099"/>
       </top>
+      <bottom/>
+      <diagonal style="thin">
+        <color theme="0"/>
+      </diagonal>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000099"/>
       </bottom>
-      <diagonal style="thin">
-        <color indexed="64"/>
-      </diagonal>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -529,7 +660,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -560,53 +691,74 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -614,6 +766,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF000099"/>
+      <color rgb="FF0000CC"/>
+      <color rgb="FF0000FF"/>
+      <color rgb="FF000066"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1213,18 +1373,18 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T13"/>
+  <dimension ref="B2:V15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="16.625" customWidth="1"/>
-    <col min="2" max="2" width="15.625" customWidth="1"/>
-    <col min="3" max="3" width="3.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.875" customWidth="1"/>
+    <col min="2" max="2" width="16.625" customWidth="1"/>
+    <col min="3" max="3" width="0.25" customWidth="1"/>
+    <col min="4" max="4" width="15.625" customWidth="1"/>
     <col min="5" max="5" width="3.375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3.375" bestFit="1" customWidth="1"/>
@@ -1241,522 +1401,560 @@
     <col min="18" max="18" width="3.5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="3.375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
-      <c r="A1" s="10"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16">
+    <row r="2" spans="2:22">
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="11">
         <v>1</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="16">
+      <c r="F2" s="11"/>
+      <c r="G2" s="11">
         <v>2</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="16">
+      <c r="H2" s="11"/>
+      <c r="I2" s="11">
         <v>3</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="16">
+      <c r="J2" s="11"/>
+      <c r="K2" s="11">
         <v>4</v>
       </c>
-      <c r="J1" s="17"/>
-      <c r="K1" s="16">
+      <c r="L2" s="11"/>
+      <c r="M2" s="11">
         <v>5</v>
       </c>
-      <c r="L1" s="17"/>
-      <c r="M1" s="16">
-        <v>6</v>
-      </c>
-      <c r="N1" s="17"/>
-      <c r="O1" s="16">
+      <c r="N2" s="11"/>
+      <c r="O2" s="11">
+        <v>6</v>
+      </c>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11">
         <v>7</v>
       </c>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="16">
+      <c r="R2" s="11"/>
+      <c r="S2" s="11">
         <v>8</v>
       </c>
-      <c r="R1" s="17"/>
-      <c r="S1" s="16">
+      <c r="T2" s="11"/>
+      <c r="U2" s="11">
         <v>9</v>
       </c>
-      <c r="T1" s="17"/>
-    </row>
-    <row r="2" spans="1:20" ht="48">
-      <c r="A2" s="25" t="s">
+      <c r="V2" s="12"/>
+    </row>
+    <row r="3" spans="2:22" ht="1.5" customHeight="1">
+      <c r="B3" s="32"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="25"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="25"/>
+      <c r="U3" s="25"/>
+      <c r="V3" s="26"/>
+    </row>
+    <row r="4" spans="2:22" ht="48">
+      <c r="B4" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="C4" s="29"/>
+      <c r="D4" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="19"/>
-    </row>
-    <row r="3" spans="1:20" ht="24">
-      <c r="A3" s="25"/>
-      <c r="B3" s="11" t="s">
+      <c r="E4" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
+      <c r="S4" s="18"/>
+      <c r="T4" s="18"/>
+      <c r="U4" s="18"/>
+      <c r="V4" s="18"/>
+    </row>
+    <row r="5" spans="2:22" ht="24">
+      <c r="B5" s="14"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="L3" s="21"/>
-      <c r="M3" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="N3" s="21"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="21"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="21"/>
-    </row>
-    <row r="4" spans="1:20" ht="24">
-      <c r="A4" s="25"/>
-      <c r="B4" s="11" t="s">
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="20"/>
+      <c r="V5" s="20"/>
+    </row>
+    <row r="6" spans="2:22" ht="24">
+      <c r="B6" s="14"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="R4" s="21"/>
-      <c r="S4" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="T4" s="21"/>
-    </row>
-    <row r="5" spans="1:20" ht="48">
-      <c r="A5" s="25" t="s">
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="T6" s="20"/>
+      <c r="U6" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="V6" s="20"/>
+    </row>
+    <row r="7" spans="2:22" ht="48">
+      <c r="B7" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="C7" s="29"/>
+      <c r="D7" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="J5" s="19"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="19"/>
-      <c r="S5" s="18"/>
-      <c r="T5" s="19"/>
-    </row>
-    <row r="6" spans="1:20" ht="24">
-      <c r="A6" s="25"/>
-      <c r="B6" s="11" t="s">
+      <c r="E7" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="R7" s="21"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="21"/>
+      <c r="U7" s="21"/>
+      <c r="V7" s="21"/>
+    </row>
+    <row r="8" spans="2:22" ht="24">
+      <c r="B8" s="14"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="L6" s="19"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="R6" s="19"/>
-      <c r="S6" s="20"/>
-      <c r="T6" s="21"/>
-    </row>
-    <row r="7" spans="1:20" ht="24">
-      <c r="A7" s="25"/>
-      <c r="B7" s="11" t="s">
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="N8" s="21"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="T8" s="21"/>
+      <c r="U8" s="20"/>
+      <c r="V8" s="20"/>
+    </row>
+    <row r="9" spans="2:22" ht="24">
+      <c r="B9" s="14"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="H7" s="21"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="N7" s="19"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="20"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="T7" s="19"/>
-    </row>
-    <row r="8" spans="1:20" ht="24">
-      <c r="A8" s="24" t="s">
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="20"/>
+      <c r="U9" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="V9" s="21"/>
+    </row>
+    <row r="10" spans="2:22" ht="24">
+      <c r="B10" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="30"/>
+      <c r="D10" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="E10" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="R10" s="22"/>
+      <c r="S10" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="T10" s="22"/>
+      <c r="U10" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="V10" s="22"/>
+    </row>
+    <row r="11" spans="2:22" ht="24">
+      <c r="B11" s="15"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="R8" s="12"/>
-      <c r="S8" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="T8" s="12"/>
-    </row>
-    <row r="9" spans="1:20" ht="24">
-      <c r="A9" s="24"/>
-      <c r="B9" s="11" t="s">
+      <c r="E11" s="23"/>
+      <c r="F11" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="U11" s="23"/>
+      <c r="V11" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22">
+      <c r="B12" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="29"/>
+      <c r="D12" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="S9" s="13"/>
-      <c r="T9" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20">
-      <c r="A10" s="22" t="s">
+      <c r="E12" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="23"/>
+      <c r="U12" s="23"/>
+      <c r="V12" s="23"/>
+    </row>
+    <row r="13" spans="2:22">
+      <c r="B13" s="14"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="E13" s="23"/>
+      <c r="F13" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="S13" s="23"/>
+      <c r="T13" s="23"/>
+      <c r="U13" s="23"/>
+      <c r="V13" s="23"/>
+    </row>
+    <row r="14" spans="2:22">
+      <c r="B14" s="14"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
-    </row>
-    <row r="11" spans="1:20">
-      <c r="A11" s="23"/>
-      <c r="B11" s="11" t="s">
+      <c r="E14" s="23"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="L14" s="23"/>
+      <c r="M14" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="N14" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="O14" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="23"/>
+      <c r="S14" s="22"/>
+      <c r="T14" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="U14" s="22"/>
+      <c r="V14" s="23"/>
+    </row>
+    <row r="15" spans="2:22">
+      <c r="B15" s="16"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="13"/>
-      <c r="T11" s="13"/>
-    </row>
-    <row r="12" spans="1:20">
-      <c r="A12" s="23"/>
-      <c r="B12" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="J12" s="13"/>
-      <c r="K12" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="L12" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="M12" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="N12" s="13"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="S12" s="12"/>
-      <c r="T12" s="13"/>
-    </row>
-    <row r="13" spans="1:20">
-      <c r="A13" s="23"/>
-      <c r="B13" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="I13" s="13"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="O13" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="R13" s="12"/>
-      <c r="S13" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="T13" s="12" t="s">
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="J15" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="K15" s="23"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q15" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="R15" s="22"/>
+      <c r="S15" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="T15" s="22"/>
+      <c r="U15" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="V15" s="22" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="I7:J7"/>
     <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="K9:L9"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="I6:J6"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="K7:L7"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K8:L8"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>